<commit_message>
picked the first 10 molecules in the excel file for the first 10 levels
</commit_message>
<xml_diff>
--- a/Documents/MoleculesOrderd.xlsx
+++ b/Documents/MoleculesOrderd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>O2</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>C3H6</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
@@ -715,18 +718,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="0.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -736,8 +740,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -748,7 +755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -759,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -770,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -781,7 +788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -792,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -803,7 +810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -813,8 +820,11 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -825,7 +835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -836,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -847,7 +857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -858,7 +868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -869,7 +879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -879,8 +889,11 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -890,8 +903,11 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -902,7 +918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -913,7 +929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -923,8 +939,11 @@
       <c r="C18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3</v>
       </c>
@@ -935,7 +954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -946,7 +965,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -957,7 +976,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -968,7 +987,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -979,7 +998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -989,8 +1008,11 @@
       <c r="C24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -1001,7 +1023,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -1011,8 +1033,11 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -1023,7 +1048,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1034,7 +1059,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -1045,7 +1070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1055,8 +1080,11 @@
       <c r="C30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -1067,7 +1095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -1077,8 +1105,11 @@
       <c r="C32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -1088,8 +1119,11 @@
       <c r="C33" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -1100,7 +1134,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -1111,7 +1145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -1122,7 +1156,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -1133,7 +1167,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1144,7 +1178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>4</v>
       </c>
@@ -1155,7 +1189,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4</v>
       </c>
@@ -1166,7 +1200,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>4</v>
       </c>
@@ -1177,7 +1211,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4</v>
       </c>
@@ -1188,7 +1222,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1199,7 +1233,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>5</v>
       </c>
@@ -1210,7 +1244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>5</v>
       </c>
@@ -1221,7 +1255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>5</v>
       </c>
@@ -1232,7 +1266,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>5</v>
       </c>
@@ -1243,7 +1277,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>5</v>
       </c>
@@ -1254,7 +1288,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>5</v>
       </c>
@@ -1264,8 +1298,11 @@
       <c r="C49" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>5</v>
       </c>
@@ -1276,7 +1313,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>5</v>
       </c>
@@ -1287,7 +1324,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1298,7 +1335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>6</v>
       </c>
@@ -1309,7 +1346,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>6</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>6</v>
       </c>
@@ -1331,7 +1368,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7</v>
       </c>
@@ -1342,7 +1379,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1353,7 +1390,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7</v>
       </c>
@@ -1364,7 +1401,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1375,7 +1412,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
updated the molecule documents
</commit_message>
<xml_diff>
--- a/Documents/MoleculesOrderd.xlsx
+++ b/Documents/MoleculesOrderd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>O2</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Hydrogen Bromide</t>
   </si>
   <si>
-    <t>IO^-1</t>
-  </si>
-  <si>
-    <t>Hypoiodite Ion</t>
-  </si>
-  <si>
     <t>HF</t>
   </si>
   <si>
@@ -54,12 +48,6 @@
     <t>ClO</t>
   </si>
   <si>
-    <t>Hypobromite Ion</t>
-  </si>
-  <si>
-    <t>BrO^-1</t>
-  </si>
-  <si>
     <t>H2</t>
   </si>
   <si>
@@ -114,48 +102,18 @@
     <t>Chlorine</t>
   </si>
   <si>
-    <t>Nitrogen Dioxide</t>
-  </si>
-  <si>
-    <t>NO2^+1</t>
-  </si>
-  <si>
     <t>Dichlorine oxide</t>
   </si>
   <si>
     <t>Cl2O</t>
   </si>
   <si>
-    <t>Bromite Ion</t>
-  </si>
-  <si>
-    <t>BrO2^-1</t>
-  </si>
-  <si>
-    <t>Chlorite Ion</t>
-  </si>
-  <si>
-    <t>ClO2^-1</t>
-  </si>
-  <si>
     <t>Hyponitrous Acid</t>
   </si>
   <si>
-    <t>Triiodide Ion</t>
-  </si>
-  <si>
     <t>HNO</t>
   </si>
   <si>
-    <t>I3^-1</t>
-  </si>
-  <si>
-    <t>Iodite Ion</t>
-  </si>
-  <si>
-    <t>IO2^-1</t>
-  </si>
-  <si>
     <t>Nitrous Oxide</t>
   </si>
   <si>
@@ -171,15 +129,9 @@
     <t>Sulfur Dioxide</t>
   </si>
   <si>
-    <t>Nitrite Ion</t>
-  </si>
-  <si>
     <t>SO2</t>
   </si>
   <si>
-    <t>NO2^-1</t>
-  </si>
-  <si>
     <t>Ethyne</t>
   </si>
   <si>
@@ -216,18 +168,6 @@
     <t>PH3</t>
   </si>
   <si>
-    <t>Carbonate Ion</t>
-  </si>
-  <si>
-    <t>CO3^-2</t>
-  </si>
-  <si>
-    <t>Nitrogen Trioxide</t>
-  </si>
-  <si>
-    <t>NO3</t>
-  </si>
-  <si>
     <t>Phosphorus Trichloride</t>
   </si>
   <si>
@@ -240,30 +180,6 @@
     <t>ClF3</t>
   </si>
   <si>
-    <t>Chlorate Ion</t>
-  </si>
-  <si>
-    <t>ClO3^-1</t>
-  </si>
-  <si>
-    <t>Iodate Ion</t>
-  </si>
-  <si>
-    <t>IO3^-1</t>
-  </si>
-  <si>
-    <t>Nitrate Ion</t>
-  </si>
-  <si>
-    <t>NO3^-1</t>
-  </si>
-  <si>
-    <t>Sulfite Ion</t>
-  </si>
-  <si>
-    <t>SO3^-2</t>
-  </si>
-  <si>
     <t>Hydrogen Peroxide</t>
   </si>
   <si>
@@ -276,24 +192,6 @@
     <t>CCl4</t>
   </si>
   <si>
-    <t>Perbromate Ion</t>
-  </si>
-  <si>
-    <t>BrO4^-1</t>
-  </si>
-  <si>
-    <t>Perchlorate Ion</t>
-  </si>
-  <si>
-    <t>ClO4^-1</t>
-  </si>
-  <si>
-    <t>Periodate Ion</t>
-  </si>
-  <si>
-    <t>IO4^-1</t>
-  </si>
-  <si>
     <t>Bromic Acid</t>
   </si>
   <si>
@@ -316,12 +214,6 @@
   </si>
   <si>
     <t>PO4^-3</t>
-  </si>
-  <si>
-    <t>Sulfate Ion</t>
-  </si>
-  <si>
-    <t>SO4^-2</t>
   </si>
   <si>
     <t>Phosphorus Pentafluoride</t>
@@ -718,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -778,14 +670,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,10 +685,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
+      <c r="E6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,21 +706,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" t="s">
@@ -867,59 +759,62 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14">
         <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" t="s">
@@ -928,9 +823,12 @@
       <c r="C17" t="s">
         <v>32</v>
       </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -938,9 +836,6 @@
       </c>
       <c r="C18" t="s">
         <v>34</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -953,10 +848,13 @@
       <c r="C19" t="s">
         <v>36</v>
       </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>3</v>
+      <c r="A20">
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -967,10 +865,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
@@ -978,18 +876,21 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
@@ -1000,7 +901,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
@@ -1009,12 +910,12 @@
         <v>46</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -1022,34 +923,34 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="E26">
-        <v>6</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>4</v>
       </c>
       <c r="B28" t="s">
@@ -1060,8 +961,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>4</v>
+      <c r="A29">
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
@@ -1072,7 +973,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -1080,13 +981,10 @@
       <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
@@ -1097,7 +995,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
@@ -1106,12 +1004,12 @@
         <v>62</v>
       </c>
       <c r="E32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
@@ -1119,13 +1017,10 @@
       <c r="C33" t="s">
         <v>64</v>
       </c>
-      <c r="E33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>4</v>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>67</v>
@@ -1134,9 +1029,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>69</v>
@@ -1145,31 +1040,31 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>4</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>7</v>
       </c>
       <c r="B38" t="s">
         <v>75</v>
@@ -1178,9 +1073,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>4</v>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
@@ -1189,9 +1084,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>4</v>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>79</v>
@@ -1200,227 +1095,26 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>4</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>8</v>
       </c>
       <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
         <v>81</v>
       </c>
-      <c r="C41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>4</v>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>9</v>
       </c>
       <c r="B42" t="s">
         <v>83</v>
       </c>
       <c r="C42" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>5</v>
-      </c>
-      <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>5</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>6</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>6</v>
-      </c>
-      <c r="B54" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>6</v>
-      </c>
-      <c r="B55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>8</v>
-      </c>
-      <c r="B59" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>9</v>
-      </c>
-      <c r="B60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C60" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All room properties finished in room_settings.ini file
</commit_message>
<xml_diff>
--- a/Documents/MoleculesOrderd.xlsx
+++ b/Documents/MoleculesOrderd.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\OneDrive\Documents\[2017]\[Spring]\AtomPuzzler\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-480" yWindow="1290" windowWidth="7395" windowHeight="3240"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>O2</t>
   </si>
@@ -271,12 +276,24 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>Dihydrogen Oxide</t>
+  </si>
+  <si>
+    <t>NaOH</t>
+  </si>
+  <si>
+    <t>Sodium Hydroxide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -318,6 +335,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -366,7 +386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,9 +419,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,6 +471,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -610,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,9 +744,6 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -759,9 +810,6 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -773,58 +821,55 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -832,10 +877,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,49 +888,49 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
+      <c r="A20" s="1">
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>4</v>
-      </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E22">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,10 +938,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,13 +949,10 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,13 +960,13 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E25">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,10 +974,13 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,10 +988,13 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,43 +1002,49 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>5</v>
+      <c r="A29" s="1">
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>5</v>
       </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>5</v>
-      </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="E31">
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,122 +1052,159 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>5</v>
       </c>
       <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>6</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>6</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>6</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
       <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
         <v>79</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>8</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>80</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>9</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>83</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>